<commit_message>
throw a sensible error when study is not found on get_study (don't 500) some ugly fixes in the file_service for improving panda output from spreadsheet processing that I need to revist. now that the spiff-workflow handles multi-instance, we can't have random multi-instance tasks around. Improved tests around study deletion.
</commit_message>
<xml_diff>
--- a/crc/static/reference/irb_documents.xlsx
+++ b/crc/static/reference/irb_documents.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="234">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -831,25 +831,25 @@
   </sheetPr>
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A99" activeCellId="0" sqref="A99"/>
+      <selection pane="bottomLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="71.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.83"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -872,7 +872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
@@ -895,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
@@ -905,14 +905,11 @@
       <c r="C3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>15</v>
       </c>
@@ -929,7 +926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>18</v>
       </c>
@@ -952,7 +949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>21</v>
       </c>
@@ -962,14 +959,11 @@
       <c r="C6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E6" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>23</v>
       </c>
@@ -979,14 +973,11 @@
       <c r="C7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E7" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>25</v>
       </c>
@@ -996,14 +987,11 @@
       <c r="C8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E8" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>27</v>
       </c>
@@ -1013,14 +1001,11 @@
       <c r="C9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E9" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>29</v>
       </c>
@@ -1030,14 +1015,11 @@
       <c r="C10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E10" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>31</v>
       </c>
@@ -1047,14 +1029,11 @@
       <c r="C11" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E11" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>33</v>
       </c>
@@ -1064,14 +1043,11 @@
       <c r="C12" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E12" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>35</v>
       </c>
@@ -1088,7 +1064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>38</v>
       </c>
@@ -1105,7 +1081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>40</v>
       </c>
@@ -1122,7 +1098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>42</v>
       </c>
@@ -1132,14 +1108,11 @@
       <c r="C16" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E16" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>44</v>
       </c>
@@ -1149,14 +1122,11 @@
       <c r="C17" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E17" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>46</v>
       </c>
@@ -1166,14 +1136,11 @@
       <c r="C18" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E18" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>48</v>
       </c>
@@ -1183,14 +1150,11 @@
       <c r="C19" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E19" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>50</v>
       </c>
@@ -1200,14 +1164,11 @@
       <c r="C20" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E20" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>52</v>
       </c>
@@ -1217,14 +1178,11 @@
       <c r="C21" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E21" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>54</v>
       </c>
@@ -1234,14 +1192,11 @@
       <c r="C22" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E22" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>56</v>
       </c>
@@ -1251,14 +1206,11 @@
       <c r="C23" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E23" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>58</v>
       </c>
@@ -1268,14 +1220,11 @@
       <c r="C24" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E24" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>60</v>
       </c>
@@ -1285,14 +1234,11 @@
       <c r="C25" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E25" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>62</v>
       </c>
@@ -1302,14 +1248,11 @@
       <c r="C26" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E26" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>65</v>
       </c>
@@ -1319,14 +1262,11 @@
       <c r="C27" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E27" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>67</v>
       </c>
@@ -1336,14 +1276,11 @@
       <c r="C28" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E28" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>69</v>
       </c>
@@ -1353,14 +1290,11 @@
       <c r="C29" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E29" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>71</v>
       </c>
@@ -1370,14 +1304,11 @@
       <c r="C30" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E30" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>74</v>
       </c>
@@ -1387,14 +1318,11 @@
       <c r="C31" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E31" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>76</v>
       </c>
@@ -1404,14 +1332,11 @@
       <c r="C32" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E32" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>78</v>
       </c>
@@ -1421,14 +1346,11 @@
       <c r="C33" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E33" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>80</v>
       </c>
@@ -1438,9 +1360,6 @@
       <c r="C34" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E34" s="0" t="s">
         <v>11</v>
       </c>
@@ -1451,7 +1370,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>83</v>
       </c>
@@ -1461,14 +1380,11 @@
       <c r="C35" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="E35" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>85</v>
       </c>
@@ -1485,7 +1401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>88</v>
       </c>
@@ -1502,7 +1418,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>90</v>
       </c>
@@ -1519,7 +1435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>92</v>
       </c>
@@ -1536,7 +1452,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>94</v>
       </c>
@@ -1559,7 +1475,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>97</v>
       </c>
@@ -1576,7 +1492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>99</v>
       </c>
@@ -1593,7 +1509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>101</v>
       </c>
@@ -1610,7 +1526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>103</v>
       </c>
@@ -1627,7 +1543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>106</v>
       </c>
@@ -1644,7 +1560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>108</v>
       </c>
@@ -1661,7 +1577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>110</v>
       </c>
@@ -1678,7 +1594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>113</v>
       </c>
@@ -1695,7 +1611,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>115</v>
       </c>
@@ -1712,7 +1628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>118</v>
       </c>
@@ -1729,7 +1645,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>120</v>
       </c>
@@ -1746,7 +1662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>122</v>
       </c>
@@ -1763,7 +1679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>124</v>
       </c>
@@ -1786,7 +1702,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>128</v>
       </c>
@@ -1809,7 +1725,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>130</v>
       </c>
@@ -1826,7 +1742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>132</v>
       </c>
@@ -1843,7 +1759,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>134</v>
       </c>
@@ -1860,7 +1776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>136</v>
       </c>
@@ -1877,7 +1793,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>140</v>
       </c>
@@ -1894,7 +1810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>142</v>
       </c>
@@ -1911,7 +1827,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>144</v>
       </c>
@@ -1928,7 +1844,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>146</v>
       </c>
@@ -1945,7 +1861,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>148</v>
       </c>
@@ -1962,7 +1878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>150</v>
       </c>
@@ -1985,7 +1901,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>153</v>
       </c>
@@ -2002,7 +1918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>155</v>
       </c>
@@ -2019,7 +1935,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>158</v>
       </c>
@@ -2036,7 +1952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>159</v>
       </c>
@@ -2053,7 +1969,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>161</v>
       </c>
@@ -2070,7 +1986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>163</v>
       </c>
@@ -2087,7 +2003,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>165</v>
       </c>
@@ -2110,7 +2026,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>169</v>
       </c>
@@ -2133,7 +2049,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>172</v>
       </c>
@@ -2150,7 +2066,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>174</v>
       </c>
@@ -2173,7 +2089,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>176</v>
       </c>
@@ -2196,7 +2112,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>179</v>
       </c>
@@ -2219,7 +2135,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>182</v>
       </c>
@@ -2242,7 +2158,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>185</v>
       </c>
@@ -2259,7 +2175,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>187</v>
       </c>
@@ -2276,7 +2192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>189</v>
       </c>
@@ -2299,7 +2215,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>192</v>
       </c>
@@ -2322,7 +2238,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>195</v>
       </c>
@@ -2345,7 +2261,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>197</v>
       </c>
@@ -2368,7 +2284,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>200</v>
       </c>
@@ -2391,7 +2307,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>203</v>
       </c>
@@ -2414,7 +2330,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>207</v>
       </c>
@@ -2437,7 +2353,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>209</v>
       </c>
@@ -2454,7 +2370,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>211</v>
       </c>
@@ -2471,7 +2387,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>213</v>
       </c>
@@ -2494,7 +2410,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>216</v>
       </c>
@@ -2517,7 +2433,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>219</v>
       </c>
@@ -2540,7 +2456,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>223</v>
       </c>
@@ -2563,7 +2479,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>226</v>
       </c>
@@ -2580,7 +2496,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>228</v>
       </c>
@@ -2597,7 +2513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>230</v>
       </c>
@@ -2614,7 +2530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>231</v>
       </c>
@@ -2631,7 +2547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>232</v>
       </c>
@@ -2648,7 +2564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>233</v>
       </c>

</xml_diff>

<commit_message>
Adds protocol script to study service
</commit_message>
<xml_diff>
--- a/crc/static/reference/irb_documents.xlsx
+++ b/crc/static/reference/irb_documents.xlsx
@@ -481,7 +481,7 @@
     <t xml:space="preserve">InfoSec Approval</t>
   </si>
   <si>
-    <t xml:space="preserve">Study_Pre-creeningQuestions</t>
+    <t xml:space="preserve">Study_Pre-ScreeningQuestions</t>
   </si>
   <si>
     <t xml:space="preserve">Pre-Screening Questions</t>
@@ -834,14 +834,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.15"/>

</xml_diff>

<commit_message>
New version of irb_documents spreadsheet, that includes the `zip_key_words` column
</commit_message>
<xml_diff>
--- a/crc/static/reference/irb_documents.xlsx
+++ b/crc/static/reference/irb_documents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1498" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1608" uniqueCount="544">
   <si>
     <t>code</t>
   </si>
@@ -1365,9 +1365,6 @@
     <t>User Guide</t>
   </si>
   <si>
-    <t>Added per Alex, no specific upload in CRC1</t>
-  </si>
-  <si>
     <t>AD_SponsorLetter</t>
   </si>
   <si>
@@ -1443,9 +1440,6 @@
     <t>Study_PreScreeningQuestions</t>
   </si>
   <si>
-    <t>PreScreening Questions</t>
-  </si>
-  <si>
     <t>Drug Device Documents</t>
   </si>
   <si>
@@ -1594,6 +1588,72 @@
   </si>
   <si>
     <t>Protocol, Application &amp; Coversheet</t>
+  </si>
+  <si>
+    <t>zip_key_words</t>
+  </si>
+  <si>
+    <t>Addendum Other</t>
+  </si>
+  <si>
+    <t>Addendum Pregnant Partner</t>
+  </si>
+  <si>
+    <t>Addendum Prisoner</t>
+  </si>
+  <si>
+    <t>Minor Assent</t>
+  </si>
+  <si>
+    <t>Annual Report IDE</t>
+  </si>
+  <si>
+    <t>Annual Report IND</t>
+  </si>
+  <si>
+    <t>Investigational Device Instruction for Use Clinician</t>
+  </si>
+  <si>
+    <t>Investigational Device Instruction for Use Patient Subject</t>
+  </si>
+  <si>
+    <t>IB</t>
+  </si>
+  <si>
+    <t>IB Addendum</t>
+  </si>
+  <si>
+    <t>IB Summary of Changes</t>
+  </si>
+  <si>
+    <t>Non-UVA IRB Application</t>
+  </si>
+  <si>
+    <t>Non-UVA IRB Reliance Agreement Request Form</t>
+  </si>
+  <si>
+    <t>Non-UVA IRB Study Protocol Coversheet</t>
+  </si>
+  <si>
+    <t>Application Department Chair Signature</t>
+  </si>
+  <si>
+    <t>Application Document with Signatures</t>
+  </si>
+  <si>
+    <t>Application Investigator Agreement</t>
+  </si>
+  <si>
+    <t>Protocol Document with Signatures</t>
+  </si>
+  <si>
+    <t>UVA SIRB Other</t>
+  </si>
+  <si>
+    <t>UVA SIRB Reliance Agreement Request Form</t>
+  </si>
+  <si>
+    <t>irb_file_id</t>
   </si>
 </sst>
 </file>
@@ -1671,7 +1731,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="546">
+  <cellStyleXfs count="608">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2207,6 +2267,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2276,7 +2398,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="546">
+  <cellStyles count="608">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2551,6 +2673,37 @@
     <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2822,6 +2975,37 @@
     <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3151,18 +3335,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA206"/>
+  <dimension ref="A1:AB206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M135" sqref="M135"/>
+      <selection pane="bottomRight" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
@@ -3175,14 +3359,17 @@
     <col min="12" max="12" width="4.83203125" style="14" customWidth="1"/>
     <col min="13" max="13" width="35.33203125" customWidth="1"/>
     <col min="14" max="14" width="3.1640625" customWidth="1"/>
-    <col min="15" max="15" width="71.6640625" customWidth="1"/>
-    <col min="16" max="16" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" customWidth="1"/>
-    <col min="19" max="1033" width="8.83203125" customWidth="1"/>
+    <col min="15" max="15" width="48" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" customWidth="1"/>
+    <col min="17" max="17" width="7.5" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="12.1640625" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" customWidth="1"/>
+    <col min="22" max="1034" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="60">
+    <row r="1" spans="1:24" ht="60">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3196,28 +3383,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>487</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>489</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>438</v>
@@ -3228,8 +3415,14 @@
       <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="14">
+      <c r="P1" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="14">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -3243,7 +3436,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -3255,11 +3448,9 @@
       <c r="M2" s="10"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="24"/>
-      <c r="W2" s="24"/>
-    </row>
-    <row r="3" spans="1:23" ht="14">
+      <c r="X2" s="24"/>
+    </row>
+    <row r="3" spans="1:24" ht="14">
       <c r="A3" t="s">
         <v>225</v>
       </c>
@@ -3273,7 +3464,7 @@
         <v>227</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -3285,11 +3476,9 @@
       <c r="M3" s="10"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="24"/>
-      <c r="W3" s="24"/>
-    </row>
-    <row r="4" spans="1:23" ht="14">
+      <c r="X3" s="24"/>
+    </row>
+    <row r="4" spans="1:24" ht="14">
       <c r="A4" t="s">
         <v>420</v>
       </c>
@@ -3303,7 +3492,7 @@
         <v>141</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -3315,11 +3504,9 @@
       <c r="M4" s="10"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="24"/>
-      <c r="W4" s="24"/>
-    </row>
-    <row r="5" spans="1:23" ht="14">
+      <c r="X4" s="24"/>
+    </row>
+    <row r="5" spans="1:24" ht="14">
       <c r="A5" t="s">
         <v>421</v>
       </c>
@@ -3333,7 +3520,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -3345,11 +3532,9 @@
       <c r="M5" s="10"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="24"/>
-      <c r="W5" s="24"/>
-    </row>
-    <row r="6" spans="1:23" ht="14">
+      <c r="X5" s="24"/>
+    </row>
+    <row r="6" spans="1:24" ht="14">
       <c r="A6" t="s">
         <v>422</v>
       </c>
@@ -3363,7 +3548,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -3375,11 +3560,9 @@
       <c r="M6" s="10"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="24"/>
-      <c r="W6" s="24"/>
-    </row>
-    <row r="7" spans="1:23" ht="14">
+      <c r="X6" s="24"/>
+    </row>
+    <row r="7" spans="1:24" ht="14">
       <c r="A7" t="s">
         <v>423</v>
       </c>
@@ -3393,7 +3576,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -3405,11 +3588,9 @@
       <c r="M7" s="10"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="24"/>
-      <c r="W7" s="24"/>
-    </row>
-    <row r="8" spans="1:23" ht="14">
+      <c r="X7" s="24"/>
+    </row>
+    <row r="8" spans="1:24" ht="14">
       <c r="A8" t="s">
         <v>424</v>
       </c>
@@ -3423,7 +3604,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
@@ -3435,11 +3616,9 @@
       <c r="M8" s="10"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="24"/>
-      <c r="W8" s="24"/>
-    </row>
-    <row r="9" spans="1:23" ht="14">
+      <c r="X8" s="24"/>
+    </row>
+    <row r="9" spans="1:24" ht="14">
       <c r="A9" t="s">
         <v>425</v>
       </c>
@@ -3453,7 +3632,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
@@ -3465,11 +3644,9 @@
       <c r="M9" s="10"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="24"/>
-      <c r="W9" s="24"/>
-    </row>
-    <row r="10" spans="1:23" ht="14">
+      <c r="X9" s="24"/>
+    </row>
+    <row r="10" spans="1:24" ht="14">
       <c r="A10" t="s">
         <v>426</v>
       </c>
@@ -3483,7 +3660,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -3495,11 +3672,9 @@
       <c r="M10" s="10"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="24"/>
-      <c r="W10" s="24"/>
-    </row>
-    <row r="11" spans="1:23" ht="14">
+      <c r="X10" s="24"/>
+    </row>
+    <row r="11" spans="1:24" ht="14">
       <c r="A11" t="s">
         <v>427</v>
       </c>
@@ -3513,7 +3688,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
@@ -3525,11 +3700,9 @@
       <c r="M11" s="10"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="24"/>
-      <c r="W11" s="24"/>
-    </row>
-    <row r="12" spans="1:23" ht="14">
+      <c r="X11" s="24"/>
+    </row>
+    <row r="12" spans="1:24" ht="14">
       <c r="A12" t="s">
         <v>428</v>
       </c>
@@ -3543,7 +3716,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -3555,11 +3728,9 @@
       <c r="M12" s="10"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="24"/>
-      <c r="W12" s="24"/>
-    </row>
-    <row r="13" spans="1:23" ht="14">
+      <c r="X12" s="24"/>
+    </row>
+    <row r="13" spans="1:24" ht="14">
       <c r="A13" t="s">
         <v>429</v>
       </c>
@@ -3573,7 +3744,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -3585,11 +3756,9 @@
       <c r="M13" s="10"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="24"/>
-      <c r="W13" s="24"/>
-    </row>
-    <row r="14" spans="1:23" ht="14">
+      <c r="X13" s="24"/>
+    </row>
+    <row r="14" spans="1:24" ht="14">
       <c r="A14" t="s">
         <v>430</v>
       </c>
@@ -3616,17 +3785,23 @@
       <c r="K14" s="15"/>
       <c r="L14" s="15"/>
       <c r="M14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" t="s">
         <v>237</v>
       </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="24"/>
-      <c r="W14" s="24"/>
-    </row>
-    <row r="15" spans="1:23" ht="14">
+      <c r="P14" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>114</v>
+      </c>
+      <c r="R14" s="14"/>
+      <c r="S14" s="24"/>
+      <c r="X14" s="24"/>
+    </row>
+    <row r="15" spans="1:24" ht="14">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -3649,7 +3824,7 @@
         <v>437</v>
       </c>
       <c r="M15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N15">
         <v>12</v>
@@ -3657,11 +3832,17 @@
       <c r="O15" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="24"/>
-      <c r="W15" s="24"/>
-    </row>
-    <row r="16" spans="1:23" ht="14">
+      <c r="P15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>88</v>
+      </c>
+      <c r="R15" s="14"/>
+      <c r="S15" s="24"/>
+      <c r="X15" s="24"/>
+    </row>
+    <row r="16" spans="1:24" ht="14">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -3684,15 +3865,21 @@
         <v>437</v>
       </c>
       <c r="M16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O16" t="s">
         <v>12</v>
       </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="24"/>
-    </row>
-    <row r="17" spans="1:18" ht="14">
+      <c r="P16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>89</v>
+      </c>
+      <c r="R16" s="14"/>
+      <c r="S16" s="24"/>
+    </row>
+    <row r="17" spans="1:19" ht="14">
       <c r="A17" t="s">
         <v>238</v>
       </c>
@@ -3715,7 +3902,7 @@
         <v>437</v>
       </c>
       <c r="M17" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N17">
         <v>39</v>
@@ -3723,10 +3910,16 @@
       <c r="O17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="24"/>
-    </row>
-    <row r="18" spans="1:18" ht="14">
+      <c r="P17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>192</v>
+      </c>
+      <c r="R17" s="14"/>
+      <c r="S17" s="24"/>
+    </row>
+    <row r="18" spans="1:19" ht="14">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -3755,18 +3948,24 @@
         <v>444</v>
       </c>
       <c r="M18" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N18">
         <v>35</v>
       </c>
       <c r="O18" t="s">
-        <v>465</v>
-      </c>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="24"/>
-    </row>
-    <row r="19" spans="1:18" ht="14">
+        <v>464</v>
+      </c>
+      <c r="P18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>178</v>
+      </c>
+      <c r="R18" s="14"/>
+      <c r="S18" s="24"/>
+    </row>
+    <row r="19" spans="1:19" ht="14">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3789,7 +3988,7 @@
         <v>437</v>
       </c>
       <c r="M19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N19">
         <v>41</v>
@@ -3797,10 +3996,16 @@
       <c r="O19" t="s">
         <v>18</v>
       </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="24"/>
-    </row>
-    <row r="20" spans="1:18" ht="14">
+      <c r="P19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="14">
+        <v>102</v>
+      </c>
+      <c r="R19" s="14"/>
+      <c r="S19" s="24"/>
+    </row>
+    <row r="20" spans="1:19" ht="14">
       <c r="A20" t="s">
         <v>239</v>
       </c>
@@ -3823,15 +4028,21 @@
         <v>437</v>
       </c>
       <c r="M20" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O20" t="s">
-        <v>466</v>
-      </c>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="24"/>
-    </row>
-    <row r="21" spans="1:18" ht="14">
+        <v>465</v>
+      </c>
+      <c r="P20" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q20" s="14">
+        <v>159</v>
+      </c>
+      <c r="R20" s="14"/>
+      <c r="S20" s="24"/>
+    </row>
+    <row r="21" spans="1:19" ht="14">
       <c r="A21" t="s">
         <v>242</v>
       </c>
@@ -3854,15 +4065,21 @@
         <v>437</v>
       </c>
       <c r="M21" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O21" t="s">
-        <v>467</v>
-      </c>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="24"/>
-    </row>
-    <row r="22" spans="1:18" ht="14">
+        <v>466</v>
+      </c>
+      <c r="P21" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q21" s="14">
+        <v>158</v>
+      </c>
+      <c r="R21" s="14"/>
+      <c r="S21" s="24"/>
+    </row>
+    <row r="22" spans="1:19" ht="14">
       <c r="A22" t="s">
         <v>244</v>
       </c>
@@ -3885,15 +4102,21 @@
         <v>437</v>
       </c>
       <c r="M22" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O22" t="s">
-        <v>468</v>
-      </c>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="24"/>
-    </row>
-    <row r="23" spans="1:18" ht="14">
+        <v>467</v>
+      </c>
+      <c r="P22" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q22" s="14">
+        <v>160</v>
+      </c>
+      <c r="R22" s="14"/>
+      <c r="S22" s="24"/>
+    </row>
+    <row r="23" spans="1:19" ht="14">
       <c r="A23" t="s">
         <v>245</v>
       </c>
@@ -3916,15 +4139,21 @@
         <v>437</v>
       </c>
       <c r="M23" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O23" t="s">
-        <v>469</v>
-      </c>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="24"/>
-    </row>
-    <row r="24" spans="1:18" ht="14">
+        <v>468</v>
+      </c>
+      <c r="P23" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q23" s="14">
+        <v>180</v>
+      </c>
+      <c r="R23" s="14"/>
+      <c r="S23" s="24"/>
+    </row>
+    <row r="24" spans="1:19" ht="14">
       <c r="A24" t="s">
         <v>247</v>
       </c>
@@ -3947,15 +4176,21 @@
         <v>437</v>
       </c>
       <c r="M24" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O24" t="s">
         <v>248</v>
       </c>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="24"/>
-    </row>
-    <row r="25" spans="1:18" ht="14">
+      <c r="P24" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q24" s="14">
+        <v>97</v>
+      </c>
+      <c r="R24" s="14"/>
+      <c r="S24" s="24"/>
+    </row>
+    <row r="25" spans="1:19" ht="14">
       <c r="A25" t="s">
         <v>249</v>
       </c>
@@ -3969,12 +4204,18 @@
         <v>9</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="24"/>
-    </row>
-    <row r="26" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+      <c r="P25" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q25" s="14">
+        <v>98</v>
+      </c>
+      <c r="R25" s="14"/>
+      <c r="S25" s="24"/>
+    </row>
+    <row r="26" spans="1:19" ht="14">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -3997,15 +4238,21 @@
         <v>437</v>
       </c>
       <c r="M26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O26" t="s">
         <v>21</v>
       </c>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="24"/>
-    </row>
-    <row r="27" spans="1:18" ht="14">
+      <c r="P26" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q26" s="14">
+        <v>101</v>
+      </c>
+      <c r="R26" s="14"/>
+      <c r="S26" s="24"/>
+    </row>
+    <row r="27" spans="1:19" ht="14">
       <c r="A27" t="s">
         <v>436</v>
       </c>
@@ -4028,15 +4275,21 @@
         <v>437</v>
       </c>
       <c r="M27" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O27" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="24"/>
-    </row>
-    <row r="28" spans="1:18" ht="14">
+      <c r="P27" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="14">
+        <v>99</v>
+      </c>
+      <c r="R27" s="14"/>
+      <c r="S27" s="24"/>
+    </row>
+    <row r="28" spans="1:19" ht="14">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -4059,15 +4312,21 @@
         <v>437</v>
       </c>
       <c r="M28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O28" t="s">
         <v>23</v>
       </c>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="24"/>
-    </row>
-    <row r="29" spans="1:18" ht="14">
+      <c r="P28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="14">
+        <v>115</v>
+      </c>
+      <c r="R28" s="14"/>
+      <c r="S28" s="24"/>
+    </row>
+    <row r="29" spans="1:19" ht="14">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -4090,15 +4349,21 @@
         <v>437</v>
       </c>
       <c r="M29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O29" t="s">
         <v>25</v>
       </c>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="24"/>
-    </row>
-    <row r="30" spans="1:18" ht="14">
+      <c r="P29" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q29" s="14">
+        <v>116</v>
+      </c>
+      <c r="R29" s="14"/>
+      <c r="S29" s="24"/>
+    </row>
+    <row r="30" spans="1:19" ht="14">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -4121,7 +4386,7 @@
         <v>437</v>
       </c>
       <c r="M30" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N30">
         <v>20</v>
@@ -4129,10 +4394,16 @@
       <c r="O30" t="s">
         <v>435</v>
       </c>
-      <c r="Q30" s="14"/>
-      <c r="R30" s="24"/>
-    </row>
-    <row r="31" spans="1:18" ht="14">
+      <c r="P30" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="14">
+        <v>103</v>
+      </c>
+      <c r="R30" s="14"/>
+      <c r="S30" s="24"/>
+    </row>
+    <row r="31" spans="1:19" ht="14">
       <c r="A31" t="s">
         <v>251</v>
       </c>
@@ -4146,12 +4417,10 @@
         <v>9</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="24"/>
-    </row>
-    <row r="32" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="14">
       <c r="A32" t="s">
         <v>253</v>
       </c>
@@ -4165,12 +4434,10 @@
         <v>9</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="24"/>
-    </row>
-    <row r="33" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="14">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -4193,15 +4460,21 @@
         <v>437</v>
       </c>
       <c r="M33" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O33" t="s">
         <v>29</v>
       </c>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="24"/>
-    </row>
-    <row r="34" spans="1:18" ht="14">
+      <c r="P33" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q33" s="14">
+        <v>117</v>
+      </c>
+      <c r="R33" s="14"/>
+      <c r="S33" s="24"/>
+    </row>
+    <row r="34" spans="1:19" ht="14">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -4224,15 +4497,21 @@
         <v>437</v>
       </c>
       <c r="M34" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O34" t="s">
         <v>31</v>
       </c>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="24"/>
-    </row>
-    <row r="35" spans="1:18" ht="14">
+      <c r="P34" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q34" s="14">
+        <v>118</v>
+      </c>
+      <c r="R34" s="14"/>
+      <c r="S34" s="24"/>
+    </row>
+    <row r="35" spans="1:19" ht="14">
       <c r="A35" t="s">
         <v>255</v>
       </c>
@@ -4255,15 +4534,21 @@
         <v>437</v>
       </c>
       <c r="M35" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O35" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="24"/>
-    </row>
-    <row r="36" spans="1:18" ht="14">
+      <c r="P35" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q35" s="14">
+        <v>119</v>
+      </c>
+      <c r="R35" s="14"/>
+      <c r="S35" s="24"/>
+    </row>
+    <row r="36" spans="1:19" ht="14">
       <c r="A36" t="s">
         <v>257</v>
       </c>
@@ -4286,15 +4571,21 @@
         <v>437</v>
       </c>
       <c r="M36" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O36" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="24"/>
-    </row>
-    <row r="37" spans="1:18" ht="14">
+      <c r="P36" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q36" s="14">
+        <v>194</v>
+      </c>
+      <c r="R36" s="14"/>
+      <c r="S36" s="24"/>
+    </row>
+    <row r="37" spans="1:19" ht="14">
       <c r="A37" t="s">
         <v>259</v>
       </c>
@@ -4317,17 +4608,23 @@
         <v>437</v>
       </c>
       <c r="M37" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O37" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="24"/>
-    </row>
-    <row r="38" spans="1:18" ht="14">
+      <c r="P37" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q37" s="14">
+        <v>195</v>
+      </c>
+      <c r="R37" s="14"/>
+      <c r="S37" s="24"/>
+    </row>
+    <row r="38" spans="1:19" ht="14">
       <c r="A38" s="19" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B38" s="19" t="s">
         <v>7</v>
@@ -4348,18 +4645,23 @@
         <v>437</v>
       </c>
       <c r="M38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O38" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="24"/>
-    </row>
-    <row r="39" spans="1:18" ht="14">
+      <c r="P38" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q38" s="14">
+        <v>209</v>
+      </c>
+      <c r="R38" s="14"/>
+      <c r="S38" s="24"/>
+    </row>
+    <row r="39" spans="1:19" ht="14">
       <c r="A39" s="19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>7</v>
@@ -4380,18 +4682,21 @@
         <v>437</v>
       </c>
       <c r="M39" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="O39" s="19" t="s">
         <v>446</v>
       </c>
-      <c r="P39" s="20" t="s">
-        <v>447</v>
-      </c>
-      <c r="Q39" s="14"/>
-      <c r="R39" s="24"/>
-    </row>
-    <row r="40" spans="1:18" ht="14">
+      <c r="P39" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>210</v>
+      </c>
+      <c r="R39" s="14"/>
+      <c r="S39" s="24"/>
+    </row>
+    <row r="40" spans="1:19" ht="14">
       <c r="A40" t="s">
         <v>434</v>
       </c>
@@ -4417,12 +4722,18 @@
         <v>442</v>
       </c>
       <c r="O40" t="s">
-        <v>463</v>
-      </c>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="24"/>
-    </row>
-    <row r="41" spans="1:18" ht="14">
+        <v>462</v>
+      </c>
+      <c r="P40" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q40" s="14">
+        <v>2</v>
+      </c>
+      <c r="R40" s="14"/>
+      <c r="S40" s="24"/>
+    </row>
+    <row r="41" spans="1:19" ht="14">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -4451,12 +4762,18 @@
         <v>442</v>
       </c>
       <c r="O41" t="s">
-        <v>478</v>
-      </c>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="24"/>
-    </row>
-    <row r="42" spans="1:18" ht="14">
+        <v>476</v>
+      </c>
+      <c r="P41" t="s">
+        <v>524</v>
+      </c>
+      <c r="Q41" s="14">
+        <v>1</v>
+      </c>
+      <c r="R41" s="14"/>
+      <c r="S41" s="24"/>
+    </row>
+    <row r="42" spans="1:19" ht="14">
       <c r="A42" t="s">
         <v>221</v>
       </c>
@@ -4485,12 +4802,18 @@
         <v>442</v>
       </c>
       <c r="O42" t="s">
-        <v>479</v>
-      </c>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="24"/>
-    </row>
-    <row r="43" spans="1:18" ht="14">
+        <v>477</v>
+      </c>
+      <c r="P42" t="s">
+        <v>523</v>
+      </c>
+      <c r="Q42" s="14">
+        <v>3</v>
+      </c>
+      <c r="R42" s="14"/>
+      <c r="S42" s="24"/>
+    </row>
+    <row r="43" spans="1:19" ht="14">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -4521,10 +4844,16 @@
       <c r="O43" t="s">
         <v>38</v>
       </c>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="24"/>
-    </row>
-    <row r="44" spans="1:18" ht="14">
+      <c r="P43" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q43" s="14">
+        <v>4</v>
+      </c>
+      <c r="R43" s="14"/>
+      <c r="S43" s="24"/>
+    </row>
+    <row r="44" spans="1:19" ht="14">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -4555,10 +4884,16 @@
       <c r="O44" t="s">
         <v>40</v>
       </c>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="24"/>
-    </row>
-    <row r="45" spans="1:18" ht="14">
+      <c r="P44" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q44" s="14">
+        <v>5</v>
+      </c>
+      <c r="R44" s="14"/>
+      <c r="S44" s="24"/>
+    </row>
+    <row r="45" spans="1:19" ht="14">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -4587,12 +4922,18 @@
         <v>442</v>
       </c>
       <c r="O45" t="s">
-        <v>480</v>
-      </c>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="24"/>
-    </row>
-    <row r="46" spans="1:18" ht="14">
+        <v>478</v>
+      </c>
+      <c r="P45" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q45" s="14">
+        <v>6</v>
+      </c>
+      <c r="R45" s="14"/>
+      <c r="S45" s="24"/>
+    </row>
+    <row r="46" spans="1:19" ht="14">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -4624,12 +4965,18 @@
         <v>39</v>
       </c>
       <c r="O46" t="s">
-        <v>493</v>
-      </c>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="24"/>
-    </row>
-    <row r="47" spans="1:18" ht="14">
+        <v>491</v>
+      </c>
+      <c r="P46" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="14">
+        <v>7</v>
+      </c>
+      <c r="R46" s="14"/>
+      <c r="S46" s="24"/>
+    </row>
+    <row r="47" spans="1:19" ht="14">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -4660,10 +5007,16 @@
       <c r="O47" t="s">
         <v>47</v>
       </c>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="24"/>
-    </row>
-    <row r="48" spans="1:18" ht="14">
+      <c r="P47" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q47" s="14">
+        <v>8</v>
+      </c>
+      <c r="R47" s="14"/>
+      <c r="S47" s="24"/>
+    </row>
+    <row r="48" spans="1:19" ht="14">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -4694,10 +5047,16 @@
       <c r="O48" t="s">
         <v>49</v>
       </c>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="24"/>
-    </row>
-    <row r="49" spans="1:18" ht="14">
+      <c r="P48" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q48" s="14">
+        <v>9</v>
+      </c>
+      <c r="R48" s="14"/>
+      <c r="S48" s="24"/>
+    </row>
+    <row r="49" spans="1:19" ht="14">
       <c r="A49" t="s">
         <v>261</v>
       </c>
@@ -4728,10 +5087,16 @@
       <c r="O49" t="s">
         <v>262</v>
       </c>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="24"/>
-    </row>
-    <row r="50" spans="1:18" ht="14">
+      <c r="P49" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q49" s="14">
+        <v>13</v>
+      </c>
+      <c r="R49" s="14"/>
+      <c r="S49" s="24"/>
+    </row>
+    <row r="50" spans="1:19" ht="14">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -4765,10 +5130,16 @@
       <c r="O50" t="s">
         <v>51</v>
       </c>
-      <c r="Q50" s="14"/>
-      <c r="R50" s="24"/>
-    </row>
-    <row r="51" spans="1:18" ht="14">
+      <c r="P50" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q50" s="14">
+        <v>10</v>
+      </c>
+      <c r="R50" s="14"/>
+      <c r="S50" s="24"/>
+    </row>
+    <row r="51" spans="1:19" ht="14">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -4799,10 +5170,16 @@
       <c r="O51" t="s">
         <v>53</v>
       </c>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="24"/>
-    </row>
-    <row r="52" spans="1:18" ht="14">
+      <c r="P51" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q51" s="14">
+        <v>11</v>
+      </c>
+      <c r="R51" s="14"/>
+      <c r="S51" s="24"/>
+    </row>
+    <row r="52" spans="1:19" ht="14">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -4830,10 +5207,16 @@
       <c r="O52" t="s">
         <v>55</v>
       </c>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="24"/>
-    </row>
-    <row r="53" spans="1:18" ht="14">
+      <c r="P52" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q52" s="14">
+        <v>12</v>
+      </c>
+      <c r="R52" s="14"/>
+      <c r="S52" s="24"/>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -4847,12 +5230,10 @@
         <v>9</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="Q53" s="14"/>
-      <c r="R53" s="24"/>
-    </row>
-    <row r="54" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -4866,12 +5247,10 @@
         <v>9</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="Q54" s="14"/>
-      <c r="R54" s="24"/>
-    </row>
-    <row r="55" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -4885,12 +5264,10 @@
         <v>9</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="24"/>
-    </row>
-    <row r="56" spans="1:18">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -4904,10 +5281,10 @@
         <v>9</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="14">
       <c r="A57" t="s">
         <v>263</v>
       </c>
@@ -4921,10 +5298,18 @@
         <v>265</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="14">
+        <v>449</v>
+      </c>
+      <c r="P57" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q57" s="14">
+        <v>68</v>
+      </c>
+      <c r="R57" s="14"/>
+      <c r="S57" s="24"/>
+    </row>
+    <row r="58" spans="1:19" ht="14">
       <c r="A58" t="s">
         <v>266</v>
       </c>
@@ -4938,10 +5323,18 @@
         <v>267</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18">
+        <v>449</v>
+      </c>
+      <c r="P58" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q58" s="14">
+        <v>69</v>
+      </c>
+      <c r="R58" s="14"/>
+      <c r="S58" s="24"/>
+    </row>
+    <row r="59" spans="1:19" ht="14">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -4970,13 +5363,21 @@
         <v>437</v>
       </c>
       <c r="M59" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O59" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="60" spans="1:18">
+      <c r="P59" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q59" s="14">
+        <v>56</v>
+      </c>
+      <c r="R59" s="14"/>
+      <c r="S59" s="24"/>
+    </row>
+    <row r="60" spans="1:19" ht="14">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -5008,13 +5409,21 @@
         <v>437</v>
       </c>
       <c r="M60" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O60" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="1:18">
+      <c r="P60" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q60" s="14">
+        <v>57</v>
+      </c>
+      <c r="R60" s="14"/>
+      <c r="S60" s="24"/>
+    </row>
+    <row r="61" spans="1:19" ht="14">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -5046,13 +5455,21 @@
         <v>437</v>
       </c>
       <c r="M61" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O61" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="62" spans="1:18">
+      <c r="P61" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q61" s="14">
+        <v>58</v>
+      </c>
+      <c r="R61" s="14"/>
+      <c r="S61" s="24"/>
+    </row>
+    <row r="62" spans="1:19" ht="14">
       <c r="A62" t="s">
         <v>72</v>
       </c>
@@ -5078,13 +5495,21 @@
         <v>437</v>
       </c>
       <c r="M62" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O62" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" ht="14">
+      <c r="P62" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q62" s="14">
+        <v>59</v>
+      </c>
+      <c r="R62" s="14"/>
+      <c r="S62" s="24"/>
+    </row>
+    <row r="63" spans="1:19" ht="14">
       <c r="A63" t="s">
         <v>268</v>
       </c>
@@ -5110,13 +5535,21 @@
         <v>437</v>
       </c>
       <c r="M63" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O63" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="14">
+        <v>473</v>
+      </c>
+      <c r="P63" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q63" s="14">
+        <v>60</v>
+      </c>
+      <c r="R63" s="14"/>
+      <c r="S63" s="24"/>
+    </row>
+    <row r="64" spans="1:19" ht="14">
       <c r="A64" t="s">
         <v>270</v>
       </c>
@@ -5142,13 +5575,21 @@
         <v>437</v>
       </c>
       <c r="M64" t="s">
+        <v>472</v>
+      </c>
+      <c r="O64" t="s">
         <v>474</v>
       </c>
-      <c r="O64" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15">
+      <c r="P64" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q64" s="14">
+        <v>61</v>
+      </c>
+      <c r="R64" s="14"/>
+      <c r="S64" s="24"/>
+    </row>
+    <row r="65" spans="1:19" ht="14">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -5180,7 +5621,7 @@
         <v>437</v>
       </c>
       <c r="M65" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N65">
         <v>1</v>
@@ -5188,8 +5629,16 @@
       <c r="O65" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="66" spans="1:15">
+      <c r="P65" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q65" s="14">
+        <v>62</v>
+      </c>
+      <c r="R65" s="14"/>
+      <c r="S65" s="24"/>
+    </row>
+    <row r="66" spans="1:19" ht="14">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -5218,13 +5667,21 @@
         <v>444</v>
       </c>
       <c r="M66" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O66" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" ht="14">
+      <c r="P66" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q66" s="14">
+        <v>63</v>
+      </c>
+      <c r="R66" s="14"/>
+      <c r="S66" s="24"/>
+    </row>
+    <row r="67" spans="1:19" ht="14">
       <c r="A67" t="s">
         <v>271</v>
       </c>
@@ -5250,13 +5707,21 @@
         <v>437</v>
       </c>
       <c r="M67" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O67" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="68" spans="1:15">
+      <c r="P67" t="s">
+        <v>533</v>
+      </c>
+      <c r="Q67" s="14">
+        <v>110</v>
+      </c>
+      <c r="R67" s="14"/>
+      <c r="S67" s="24"/>
+    </row>
+    <row r="68" spans="1:19" ht="14">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -5282,13 +5747,21 @@
         <v>437</v>
       </c>
       <c r="M68" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O68" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="69" spans="1:15">
+      <c r="P68" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q68" s="14">
+        <v>70</v>
+      </c>
+      <c r="R68" s="14"/>
+      <c r="S68" s="24"/>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -5314,13 +5787,13 @@
         <v>437</v>
       </c>
       <c r="M69" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O69" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:19" ht="14">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -5346,7 +5819,7 @@
         <v>437</v>
       </c>
       <c r="M70" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N70">
         <v>52</v>
@@ -5354,8 +5827,16 @@
       <c r="O70" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="71" spans="1:15">
+      <c r="P70" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q70" s="14">
+        <v>65</v>
+      </c>
+      <c r="R70" s="14"/>
+      <c r="S70" s="24"/>
+    </row>
+    <row r="71" spans="1:19" ht="14">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -5381,13 +5862,21 @@
         <v>437</v>
       </c>
       <c r="M71" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O71" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="72" spans="1:15">
+      <c r="P71" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q71" s="14">
+        <v>66</v>
+      </c>
+      <c r="R71" s="14"/>
+      <c r="S71" s="24"/>
+    </row>
+    <row r="72" spans="1:19" ht="14">
       <c r="A72" t="s">
         <v>90</v>
       </c>
@@ -5413,13 +5902,21 @@
         <v>437</v>
       </c>
       <c r="M72" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O72" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="73" spans="1:15">
+      <c r="P72" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q72" s="14">
+        <v>71</v>
+      </c>
+      <c r="R72" s="14"/>
+      <c r="S72" s="24"/>
+    </row>
+    <row r="73" spans="1:19" ht="14">
       <c r="A73" t="s">
         <v>92</v>
       </c>
@@ -5445,13 +5942,21 @@
         <v>437</v>
       </c>
       <c r="M73" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="O73" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" ht="14">
+      <c r="P73" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q73" s="14">
+        <v>67</v>
+      </c>
+      <c r="R73" s="14"/>
+      <c r="S73" s="24"/>
+    </row>
+    <row r="74" spans="1:19" ht="14">
       <c r="A74" t="s">
         <v>273</v>
       </c>
@@ -5465,10 +5970,10 @@
         <v>9</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="14">
       <c r="A75" t="s">
         <v>275</v>
       </c>
@@ -5482,10 +5987,16 @@
         <v>277</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+      <c r="P75" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q75">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" ht="14">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -5499,10 +6010,10 @@
         <v>9</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -5525,13 +6036,19 @@
         <v>437</v>
       </c>
       <c r="M77" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="O77" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="78" spans="1:15">
+      <c r="P77" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q77">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
       <c r="A78" t="s">
         <v>97</v>
       </c>
@@ -5545,10 +6062,10 @@
         <v>9</v>
       </c>
       <c r="E78" s="20" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" ht="14">
       <c r="A79" t="s">
         <v>280</v>
       </c>
@@ -5571,13 +6088,13 @@
         <v>437</v>
       </c>
       <c r="M79" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="O79" s="6" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="14">
+    <row r="80" spans="1:19" ht="14">
       <c r="A80" t="s">
         <v>282</v>
       </c>
@@ -5591,10 +6108,10 @@
         <v>9</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="81" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" ht="14">
       <c r="A81" t="s">
         <v>284</v>
       </c>
@@ -5608,10 +6125,10 @@
         <v>9</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="82" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" ht="14">
       <c r="A82" t="s">
         <v>286</v>
       </c>
@@ -5625,10 +6142,10 @@
         <v>9</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="83" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" ht="14">
       <c r="A83" t="s">
         <v>288</v>
       </c>
@@ -5642,10 +6159,10 @@
         <v>290</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="84" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" ht="14">
       <c r="A84" t="s">
         <v>291</v>
       </c>
@@ -5659,10 +6176,10 @@
         <v>292</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="85" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" ht="14">
       <c r="A85" t="s">
         <v>293</v>
       </c>
@@ -5676,10 +6193,10 @@
         <v>277</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="86" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" ht="14">
       <c r="A86" t="s">
         <v>294</v>
       </c>
@@ -5693,10 +6210,10 @@
         <v>295</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="87" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="87" spans="1:28" ht="14">
       <c r="A87" t="s">
         <v>296</v>
       </c>
@@ -5710,10 +6227,10 @@
         <v>297</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="88" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="88" spans="1:28" ht="14">
       <c r="A88" t="s">
         <v>298</v>
       </c>
@@ -5727,10 +6244,10 @@
         <v>9</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="89" spans="1:27" s="4" customFormat="1" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="89" spans="1:28" s="4" customFormat="1" ht="14">
       <c r="A89" t="s">
         <v>300</v>
       </c>
@@ -5744,7 +6261,7 @@
         <v>9</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F89" s="14"/>
       <c r="G89" s="14"/>
@@ -5756,9 +6273,9 @@
       <c r="M89"/>
       <c r="N89"/>
       <c r="O89"/>
-      <c r="AA89"/>
-    </row>
-    <row r="90" spans="1:27" ht="14">
+      <c r="AB89"/>
+    </row>
+    <row r="90" spans="1:28" ht="14">
       <c r="A90" t="s">
         <v>302</v>
       </c>
@@ -5772,10 +6289,10 @@
         <v>9</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="91" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="91" spans="1:28" ht="14">
       <c r="A91" t="s">
         <v>304</v>
       </c>
@@ -5789,10 +6306,10 @@
         <v>9</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="92" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="92" spans="1:28" ht="14">
       <c r="A92" t="s">
         <v>306</v>
       </c>
@@ -5806,10 +6323,10 @@
         <v>9</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="93" spans="1:27">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="93" spans="1:28">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -5832,7 +6349,7 @@
         <v>437</v>
       </c>
       <c r="M93" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="N93">
         <v>56</v>
@@ -5840,8 +6357,14 @@
       <c r="O93" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="94" spans="1:27" ht="14">
+      <c r="P93" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q93">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:28" ht="14">
       <c r="A94" t="s">
         <v>308</v>
       </c>
@@ -5855,10 +6378,10 @@
         <v>9</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="95" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" ht="14">
       <c r="A95" t="s">
         <v>310</v>
       </c>
@@ -5872,10 +6395,10 @@
         <v>9</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="96" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" ht="14">
       <c r="A96" t="s">
         <v>313</v>
       </c>
@@ -5889,10 +6412,10 @@
         <v>9</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="97" spans="1:27" s="4" customFormat="1" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="97" spans="1:28" s="4" customFormat="1" ht="14">
       <c r="A97" t="s">
         <v>315</v>
       </c>
@@ -5906,7 +6429,7 @@
         <v>9</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F97" s="14"/>
       <c r="G97" s="14"/>
@@ -5918,9 +6441,9 @@
       <c r="M97"/>
       <c r="N97"/>
       <c r="O97"/>
-      <c r="AA97"/>
-    </row>
-    <row r="98" spans="1:27" s="4" customFormat="1" ht="14">
+      <c r="AB97"/>
+    </row>
+    <row r="98" spans="1:28" s="4" customFormat="1" ht="14">
       <c r="A98" t="s">
         <v>317</v>
       </c>
@@ -5934,7 +6457,7 @@
         <v>9</v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F98" s="14"/>
       <c r="G98" s="14"/>
@@ -5946,9 +6469,9 @@
       <c r="M98"/>
       <c r="N98"/>
       <c r="O98"/>
-      <c r="AA98"/>
-    </row>
-    <row r="99" spans="1:27" ht="14">
+      <c r="AB98"/>
+    </row>
+    <row r="99" spans="1:28" ht="14">
       <c r="A99" t="s">
         <v>318</v>
       </c>
@@ -5962,10 +6485,10 @@
         <v>9</v>
       </c>
       <c r="E99" s="19" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="100" spans="1:27" s="5" customFormat="1" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28" s="5" customFormat="1" ht="14">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -5979,7 +6502,7 @@
         <v>9</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F100" s="14"/>
       <c r="G100" s="14"/>
@@ -5991,9 +6514,9 @@
       <c r="M100"/>
       <c r="N100"/>
       <c r="O100"/>
-      <c r="AA100"/>
-    </row>
-    <row r="101" spans="1:27" s="5" customFormat="1" ht="14">
+      <c r="AB100"/>
+    </row>
+    <row r="101" spans="1:28" s="5" customFormat="1" ht="14">
       <c r="A101" t="s">
         <v>320</v>
       </c>
@@ -6007,7 +6530,7 @@
         <v>9</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F101" s="14"/>
       <c r="G101" s="14"/>
@@ -6019,9 +6542,9 @@
       <c r="M101"/>
       <c r="N101"/>
       <c r="O101"/>
-      <c r="AA101"/>
-    </row>
-    <row r="102" spans="1:27" ht="14">
+      <c r="AB101"/>
+    </row>
+    <row r="102" spans="1:28" ht="14">
       <c r="A102" t="s">
         <v>323</v>
       </c>
@@ -6035,10 +6558,10 @@
         <v>9</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="103" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="103" spans="1:28" ht="14">
       <c r="A103" t="s">
         <v>325</v>
       </c>
@@ -6052,10 +6575,10 @@
         <v>9</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="104" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" ht="14">
       <c r="A104" t="s">
         <v>327</v>
       </c>
@@ -6069,10 +6592,10 @@
         <v>9</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="105" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" ht="14">
       <c r="A105" t="s">
         <v>329</v>
       </c>
@@ -6086,10 +6609,10 @@
         <v>9</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="106" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" ht="14">
       <c r="A106" t="s">
         <v>331</v>
       </c>
@@ -6103,10 +6626,10 @@
         <v>9</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="107" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" ht="14">
       <c r="A107" t="s">
         <v>333</v>
       </c>
@@ -6120,10 +6643,10 @@
         <v>289</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="108" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" ht="14">
       <c r="A108" t="s">
         <v>335</v>
       </c>
@@ -6137,10 +6660,10 @@
         <v>336</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="109" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="109" spans="1:28" ht="14">
       <c r="A109" t="s">
         <v>337</v>
       </c>
@@ -6154,10 +6677,10 @@
         <v>9</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="110" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="110" spans="1:28" ht="14">
       <c r="A110" t="s">
         <v>339</v>
       </c>
@@ -6171,10 +6694,10 @@
         <v>9</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="111" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" ht="14">
       <c r="A111" t="s">
         <v>341</v>
       </c>
@@ -6188,10 +6711,10 @@
         <v>9</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="112" spans="1:27" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="112" spans="1:28" ht="14">
       <c r="A112" t="s">
         <v>343</v>
       </c>
@@ -6205,10 +6728,10 @@
         <v>345</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" ht="14">
       <c r="A113" t="s">
         <v>346</v>
       </c>
@@ -6222,10 +6745,10 @@
         <v>347</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" ht="14">
       <c r="A114" s="6" t="s">
         <v>348</v>
       </c>
@@ -6239,10 +6762,10 @@
         <v>349</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="115" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" ht="14">
       <c r="A115" s="6" t="s">
         <v>350</v>
       </c>
@@ -6256,10 +6779,10 @@
         <v>351</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="116" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" ht="14">
       <c r="A116" s="6" t="s">
         <v>352</v>
       </c>
@@ -6273,10 +6796,10 @@
         <v>353</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" ht="14">
       <c r="A117" t="s">
         <v>354</v>
       </c>
@@ -6290,10 +6813,10 @@
         <v>9</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" ht="14">
       <c r="A118" t="s">
         <v>356</v>
       </c>
@@ -6307,10 +6830,10 @@
         <v>9</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" ht="14">
       <c r="A119" t="s">
         <v>358</v>
       </c>
@@ -6324,10 +6847,10 @@
         <v>360</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" ht="14">
       <c r="A120" t="s">
         <v>361</v>
       </c>
@@ -6341,10 +6864,10 @@
         <v>362</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="121" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" ht="14">
       <c r="A121" t="s">
         <v>363</v>
       </c>
@@ -6358,10 +6881,10 @@
         <v>9</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" ht="14">
       <c r="A122" t="s">
         <v>365</v>
       </c>
@@ -6375,10 +6898,10 @@
         <v>9</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="123" spans="1:15">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17">
       <c r="A123" t="s">
         <v>104</v>
       </c>
@@ -6401,13 +6924,19 @@
         <v>444</v>
       </c>
       <c r="M123" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="O123" s="13" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="124" spans="1:15">
+      <c r="P123" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q123">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17">
       <c r="A124" t="s">
         <v>107</v>
       </c>
@@ -6427,13 +6956,19 @@
         <v>437</v>
       </c>
       <c r="M124" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O124" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="125" spans="1:15">
+      <c r="P124" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q124">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
       <c r="A125" t="s">
         <v>109</v>
       </c>
@@ -6453,13 +6988,13 @@
         <v>437</v>
       </c>
       <c r="M125" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O125" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:17">
       <c r="A126" t="s">
         <v>111</v>
       </c>
@@ -6479,13 +7014,13 @@
         <v>437</v>
       </c>
       <c r="M126" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O126" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="14">
+    <row r="127" spans="1:17" ht="14">
       <c r="A127" t="s">
         <v>367</v>
       </c>
@@ -6499,10 +7034,10 @@
         <v>9</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="128" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" ht="14">
       <c r="A128" t="s">
         <v>369</v>
       </c>
@@ -6522,7 +7057,7 @@
         <v>437</v>
       </c>
       <c r="M128" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="N128">
         <v>47</v>
@@ -6530,8 +7065,14 @@
       <c r="O128" s="6" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="129" spans="1:21">
+      <c r="P128" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q128">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
       <c r="A129" t="s">
         <v>113</v>
       </c>
@@ -6551,13 +7092,13 @@
         <v>437</v>
       </c>
       <c r="M129" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O129" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="130" spans="1:21">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17">
       <c r="A130" t="s">
         <v>117</v>
       </c>
@@ -6577,13 +7118,13 @@
         <v>437</v>
       </c>
       <c r="M130" t="s">
+        <v>479</v>
+      </c>
+      <c r="O130" t="s">
         <v>481</v>
       </c>
-      <c r="O130" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="131" spans="1:21" ht="14">
+    </row>
+    <row r="131" spans="1:17" ht="14">
       <c r="A131" t="s">
         <v>372</v>
       </c>
@@ -6597,10 +7138,16 @@
         <v>9</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="132" spans="1:21">
+        <v>449</v>
+      </c>
+      <c r="P131" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q131">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
       <c r="A132" t="s">
         <v>119</v>
       </c>
@@ -6620,13 +7167,13 @@
         <v>437</v>
       </c>
       <c r="M132" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O132" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="133" spans="1:21">
+    <row r="133" spans="1:17">
       <c r="A133" t="s">
         <v>121</v>
       </c>
@@ -6646,7 +7193,7 @@
         <v>437</v>
       </c>
       <c r="M133" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="N133">
         <v>53</v>
@@ -6654,10 +7201,16 @@
       <c r="O133" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="134" spans="1:21" ht="14">
+      <c r="P133" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q133">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" ht="14">
       <c r="A134" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B134" t="s">
         <v>105</v>
@@ -6675,13 +7228,19 @@
         <v>437</v>
       </c>
       <c r="M134" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="O134" s="6" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="135" spans="1:21">
+      <c r="P134" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q134">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17">
       <c r="A135" s="18" t="s">
         <v>123</v>
       </c>
@@ -6704,13 +7263,19 @@
         <v>444</v>
       </c>
       <c r="M135" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="O135" s="13" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="136" spans="1:21" ht="14">
+      <c r="P135" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q135">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" ht="14">
       <c r="A136" t="s">
         <v>375</v>
       </c>
@@ -6724,10 +7289,10 @@
         <v>9</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="137" spans="1:21" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" ht="14">
       <c r="A137" t="s">
         <v>377</v>
       </c>
@@ -6741,10 +7306,10 @@
         <v>9</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="138" spans="1:21" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" ht="14">
       <c r="A138" t="s">
         <v>380</v>
       </c>
@@ -6758,10 +7323,10 @@
         <v>382</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="139" spans="1:21" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" ht="14">
       <c r="A139" t="s">
         <v>383</v>
       </c>
@@ -6775,10 +7340,10 @@
         <v>384</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="140" spans="1:21" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" ht="14">
       <c r="A140" t="s">
         <v>385</v>
       </c>
@@ -6792,10 +7357,10 @@
         <v>382</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="141" spans="1:21" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" ht="14">
       <c r="A141" t="s">
         <v>387</v>
       </c>
@@ -6809,11 +7374,10 @@
         <v>384</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>450</v>
-      </c>
-      <c r="U141" s="18"/>
-    </row>
-    <row r="142" spans="1:21">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17">
       <c r="A142" t="s">
         <v>125</v>
       </c>
@@ -6837,10 +7401,16 @@
       </c>
       <c r="M142" s="13"/>
       <c r="O142" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="143" spans="1:21">
+        <v>482</v>
+      </c>
+      <c r="P142" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q142">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17">
       <c r="A143" t="s">
         <v>129</v>
       </c>
@@ -6863,13 +7433,19 @@
         <v>444</v>
       </c>
       <c r="M143" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="O143" s="13" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="144" spans="1:21">
+        <v>483</v>
+      </c>
+      <c r="P143" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q143">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17">
       <c r="A144" t="s">
         <v>131</v>
       </c>
@@ -6895,10 +7471,16 @@
         <v>443</v>
       </c>
       <c r="O144" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="145" spans="1:15">
+        <v>469</v>
+      </c>
+      <c r="P144" t="s">
+        <v>538</v>
+      </c>
+      <c r="Q144">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17">
       <c r="A145" t="s">
         <v>133</v>
       </c>
@@ -6922,10 +7504,16 @@
       </c>
       <c r="M145" s="13"/>
       <c r="O145" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15" ht="14">
+        <v>470</v>
+      </c>
+      <c r="P145" t="s">
+        <v>539</v>
+      </c>
+      <c r="Q145">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" ht="14">
       <c r="A146" t="s">
         <v>388</v>
       </c>
@@ -6939,11 +7527,11 @@
         <v>9</v>
       </c>
       <c r="E146" s="19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M146" s="13"/>
     </row>
-    <row r="147" spans="1:15" ht="14">
+    <row r="147" spans="1:17" ht="14">
       <c r="A147" t="s">
         <v>389</v>
       </c>
@@ -6971,8 +7559,14 @@
       <c r="O147" s="6" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" ht="14">
+      <c r="P147" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q147">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" ht="14">
       <c r="A148" t="s">
         <v>391</v>
       </c>
@@ -7003,8 +7597,14 @@
       <c r="O148" s="8" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" ht="14">
+      <c r="P148" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q148">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" ht="14">
       <c r="A149" t="s">
         <v>393</v>
       </c>
@@ -7018,11 +7618,11 @@
         <v>9</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M149" s="13"/>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:17">
       <c r="A150" t="s">
         <v>135</v>
       </c>
@@ -7045,13 +7645,19 @@
         <v>444</v>
       </c>
       <c r="M150" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="O150" s="13" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="151" spans="1:15">
+      <c r="P150" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q150">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17">
       <c r="A151" t="s">
         <v>137</v>
       </c>
@@ -7073,8 +7679,14 @@
       <c r="O151" s="13" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" ht="14">
+      <c r="P151" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q151">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" ht="14">
       <c r="A152" t="s">
         <v>395</v>
       </c>
@@ -7102,8 +7714,14 @@
       <c r="O152" s="6" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" ht="14">
+      <c r="P152" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q152">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" ht="14">
       <c r="A153" t="s">
         <v>397</v>
       </c>
@@ -7132,15 +7750,15 @@
         <v>398</v>
       </c>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:17">
       <c r="A154" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B154" t="s">
         <v>126</v>
       </c>
       <c r="C154" t="s">
-        <v>473</v>
+        <v>139</v>
       </c>
       <c r="D154" t="s">
         <v>9</v>
@@ -7160,8 +7778,14 @@
       <c r="O154" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="155" spans="1:15">
+      <c r="P154" t="s">
+        <v>139</v>
+      </c>
+      <c r="Q154">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17">
       <c r="A155" t="s">
         <v>140</v>
       </c>
@@ -7187,10 +7811,16 @@
         <v>443</v>
       </c>
       <c r="O155" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="156" spans="1:15">
+        <v>490</v>
+      </c>
+      <c r="P155" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q155">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17">
       <c r="A156" t="s">
         <v>143</v>
       </c>
@@ -7219,7 +7849,7 @@
         <v>444</v>
       </c>
       <c r="M156" s="13" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="N156">
         <v>3</v>
@@ -7227,8 +7857,14 @@
       <c r="O156" s="13" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" ht="14">
+      <c r="P156" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q156">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" ht="14">
       <c r="A157" t="s">
         <v>399</v>
       </c>
@@ -7254,10 +7890,16 @@
         <v>443</v>
       </c>
       <c r="O157" s="23" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="158" spans="1:15">
+        <v>489</v>
+      </c>
+      <c r="P157" t="s">
+        <v>540</v>
+      </c>
+      <c r="Q157">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17">
       <c r="A158" t="s">
         <v>144</v>
       </c>
@@ -7285,8 +7927,14 @@
       <c r="O158" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" ht="14">
+      <c r="P158" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q158">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" ht="14">
       <c r="A159" t="s">
         <v>400</v>
       </c>
@@ -7314,8 +7962,14 @@
       <c r="O159" s="6" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="160" spans="1:15">
+      <c r="P159" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q159">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17">
       <c r="A160" t="s">
         <v>146</v>
       </c>
@@ -7346,8 +8000,14 @@
       <c r="O160" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="161" spans="1:15">
+      <c r="P160" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q160">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="161" spans="1:22">
       <c r="A161" t="s">
         <v>148</v>
       </c>
@@ -7379,10 +8039,16 @@
         <v>443</v>
       </c>
       <c r="O161" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="162" spans="1:15">
+        <v>488</v>
+      </c>
+      <c r="P161" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q161">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="162" spans="1:22">
       <c r="A162" t="s">
         <v>150</v>
       </c>
@@ -7419,8 +8085,14 @@
       <c r="O162" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="163" spans="1:15">
+      <c r="P162" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q162">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="163" spans="1:22">
       <c r="A163" t="s">
         <v>154</v>
       </c>
@@ -7457,8 +8129,14 @@
       <c r="O163" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="164" spans="1:15">
+      <c r="P163" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q163">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="164" spans="1:22">
       <c r="A164" t="s">
         <v>157</v>
       </c>
@@ -7495,8 +8173,14 @@
       <c r="O164" s="2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="165" spans="1:15">
+      <c r="P164" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q164">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="165" spans="1:22">
       <c r="A165" t="s">
         <v>159</v>
       </c>
@@ -7533,8 +8217,14 @@
       <c r="O165" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="166" spans="1:15">
+      <c r="P165" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q165">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="166" spans="1:22">
       <c r="A166" t="s">
         <v>161</v>
       </c>
@@ -7571,8 +8261,14 @@
       <c r="O166" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="167" spans="1:15">
+      <c r="P166" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q166">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="167" spans="1:22">
       <c r="A167" t="s">
         <v>164</v>
       </c>
@@ -7601,7 +8297,7 @@
         <v>444</v>
       </c>
       <c r="M167" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="N167">
         <v>32</v>
@@ -7609,8 +8305,14 @@
       <c r="O167" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:15">
+      <c r="P167" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q167">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="168" spans="1:22">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -7647,8 +8349,19 @@
       <c r="O168" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="169" spans="1:15" ht="14">
+      <c r="P168" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q168" s="4">
+        <v>130</v>
+      </c>
+      <c r="R168" s="4"/>
+      <c r="S168" s="4"/>
+      <c r="T168" s="4"/>
+      <c r="U168" s="4"/>
+      <c r="V168" s="4"/>
+    </row>
+    <row r="169" spans="1:22" ht="14">
       <c r="A169" t="s">
         <v>402</v>
       </c>
@@ -7662,10 +8375,16 @@
         <v>9</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="170" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+      <c r="P169" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q169">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="170" spans="1:22" ht="14">
       <c r="A170" t="s">
         <v>404</v>
       </c>
@@ -7694,7 +8413,7 @@
         <v>444</v>
       </c>
       <c r="M170" s="13" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N170">
         <v>57</v>
@@ -7702,8 +8421,14 @@
       <c r="O170" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="171" spans="1:15" ht="14">
+      <c r="P170" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q170">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="171" spans="1:22" ht="14">
       <c r="A171" t="s">
         <v>406</v>
       </c>
@@ -7732,13 +8457,19 @@
         <v>444</v>
       </c>
       <c r="M171" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="O171" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="172" spans="1:15">
+        <v>512</v>
+      </c>
+      <c r="P171" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q171">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="172" spans="1:22">
       <c r="A172" t="s">
         <v>170</v>
       </c>
@@ -7775,8 +8506,14 @@
       <c r="O172" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="173" spans="1:15">
+      <c r="P172" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q172">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="173" spans="1:22">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -7805,7 +8542,7 @@
         <v>444</v>
       </c>
       <c r="M173" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N173">
         <v>21</v>
@@ -7813,8 +8550,14 @@
       <c r="O173" s="2" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="174" spans="1:15">
+      <c r="P173" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q173">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="174" spans="1:22">
       <c r="A174" t="s">
         <v>174</v>
       </c>
@@ -7851,8 +8594,14 @@
       <c r="O174" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="175" spans="1:15">
+      <c r="P174" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q174">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="175" spans="1:22">
       <c r="A175" t="s">
         <v>177</v>
       </c>
@@ -7887,10 +8636,16 @@
         <v>10</v>
       </c>
       <c r="O175" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="176" spans="1:15">
+        <v>517</v>
+      </c>
+      <c r="P175" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q175">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="176" spans="1:22">
       <c r="A176" t="s">
         <v>179</v>
       </c>
@@ -7927,8 +8682,19 @@
       <c r="O176" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="177" spans="1:15">
+      <c r="P176" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q176" s="4">
+        <v>171</v>
+      </c>
+      <c r="R176" s="4"/>
+      <c r="S176" s="4"/>
+      <c r="T176" s="4"/>
+      <c r="U176" s="4"/>
+      <c r="V176" s="4"/>
+    </row>
+    <row r="177" spans="1:22">
       <c r="A177" t="s">
         <v>181</v>
       </c>
@@ -7957,7 +8723,7 @@
         <v>444</v>
       </c>
       <c r="M177" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="N177">
         <v>40</v>
@@ -7965,8 +8731,19 @@
       <c r="O177" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="178" spans="1:15">
+      <c r="P177" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q177" s="4">
+        <v>127</v>
+      </c>
+      <c r="R177" s="4"/>
+      <c r="S177" s="4"/>
+      <c r="T177" s="4"/>
+      <c r="U177" s="4"/>
+      <c r="V177" s="4"/>
+    </row>
+    <row r="178" spans="1:22">
       <c r="A178" t="s">
         <v>184</v>
       </c>
@@ -7980,7 +8757,7 @@
         <v>9</v>
       </c>
       <c r="E178" s="20" t="s">
-        <v>520</v>
+        <v>153</v>
       </c>
       <c r="F178" s="14" t="s">
         <v>437</v>
@@ -7995,7 +8772,7 @@
         <v>444</v>
       </c>
       <c r="M178" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="N178">
         <v>25</v>
@@ -8003,8 +8780,14 @@
       <c r="O178" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="179" spans="1:15">
+      <c r="P178" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q178">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="179" spans="1:22">
       <c r="A179" t="s">
         <v>187</v>
       </c>
@@ -8018,7 +8801,7 @@
         <v>189</v>
       </c>
       <c r="E179" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N179">
         <v>8</v>
@@ -8026,8 +8809,19 @@
       <c r="O179" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="180" spans="1:15">
+      <c r="P179" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q179" s="5">
+        <v>137</v>
+      </c>
+      <c r="R179" s="5"/>
+      <c r="S179" s="5"/>
+      <c r="T179" s="5"/>
+      <c r="U179" s="5"/>
+      <c r="V179" s="5"/>
+    </row>
+    <row r="180" spans="1:22">
       <c r="A180" t="s">
         <v>191</v>
       </c>
@@ -8041,7 +8835,7 @@
         <v>192</v>
       </c>
       <c r="E180" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N180">
         <v>8</v>
@@ -8049,8 +8843,19 @@
       <c r="O180" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="181" spans="1:15">
+      <c r="P180" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q180" s="5">
+        <v>136</v>
+      </c>
+      <c r="R180" s="5"/>
+      <c r="S180" s="5"/>
+      <c r="T180" s="5"/>
+      <c r="U180" s="5"/>
+      <c r="V180" s="5"/>
+    </row>
+    <row r="181" spans="1:22">
       <c r="A181" s="4" t="s">
         <v>193</v>
       </c>
@@ -8064,7 +8869,7 @@
         <v>194</v>
       </c>
       <c r="E181" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F181" s="16"/>
       <c r="G181" s="16"/>
@@ -8080,8 +8885,14 @@
       <c r="O181" s="7" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="182" spans="1:15">
+      <c r="P181" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q181">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="182" spans="1:22">
       <c r="A182" t="s">
         <v>195</v>
       </c>
@@ -8095,10 +8906,16 @@
         <v>196</v>
       </c>
       <c r="E182" s="20" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="183" spans="1:15">
+        <v>518</v>
+      </c>
+      <c r="P182" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q182">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="183" spans="1:22">
       <c r="A183" t="s">
         <v>197</v>
       </c>
@@ -8112,7 +8929,7 @@
         <v>198</v>
       </c>
       <c r="E183" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N183">
         <v>43</v>
@@ -8120,8 +8937,14 @@
       <c r="O183" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="184" spans="1:15">
+      <c r="P183" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q183">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="184" spans="1:22">
       <c r="A184" t="s">
         <v>199</v>
       </c>
@@ -8135,7 +8958,7 @@
         <v>200</v>
       </c>
       <c r="E184" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N184">
         <v>18</v>
@@ -8143,10 +8966,16 @@
       <c r="O184" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="185" spans="1:15" ht="14">
+      <c r="P184" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q184">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="185" spans="1:22" ht="14">
       <c r="A185" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B185" s="6" t="s">
         <v>151</v>
@@ -8158,10 +8987,16 @@
         <v>408</v>
       </c>
       <c r="E185" s="20" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="186" spans="1:15">
+        <v>518</v>
+      </c>
+      <c r="P185" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q185">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="186" spans="1:22">
       <c r="A186" t="s">
         <v>202</v>
       </c>
@@ -8175,7 +9010,7 @@
         <v>204</v>
       </c>
       <c r="E186" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N186">
         <v>22</v>
@@ -8183,8 +9018,14 @@
       <c r="O186" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="187" spans="1:15">
+      <c r="P186" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q186">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="187" spans="1:22">
       <c r="A187" t="s">
         <v>206</v>
       </c>
@@ -8198,7 +9039,7 @@
         <v>207</v>
       </c>
       <c r="E187" s="20" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="N187">
         <v>23</v>
@@ -8206,8 +9047,14 @@
       <c r="O187" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="188" spans="1:15">
+      <c r="P187" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q187">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="188" spans="1:22">
       <c r="A188" t="s">
         <v>209</v>
       </c>
@@ -8221,10 +9068,16 @@
         <v>9</v>
       </c>
       <c r="E188" s="20" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="189" spans="1:15">
+        <v>518</v>
+      </c>
+      <c r="P188" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q188">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="189" spans="1:22">
       <c r="A189" t="s">
         <v>211</v>
       </c>
@@ -8238,10 +9091,10 @@
         <v>9</v>
       </c>
       <c r="E189" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="190" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="190" spans="1:22" ht="14">
       <c r="A190" t="s">
         <v>409</v>
       </c>
@@ -8255,10 +9108,10 @@
         <v>9</v>
       </c>
       <c r="E190" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="191" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="191" spans="1:22" ht="14">
       <c r="A191" t="s">
         <v>411</v>
       </c>
@@ -8272,10 +9125,16 @@
         <v>9</v>
       </c>
       <c r="E191" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="192" spans="1:15" ht="14">
+        <v>449</v>
+      </c>
+      <c r="P191" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q191">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="192" spans="1:22" ht="14">
       <c r="A192" t="s">
         <v>412</v>
       </c>
@@ -8289,7 +9148,13 @@
         <v>9</v>
       </c>
       <c r="E192" t="s">
-        <v>450</v>
+        <v>449</v>
+      </c>
+      <c r="P192" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q192">
+        <v>154</v>
       </c>
     </row>
     <row r="193" spans="1:15">
@@ -8306,7 +9171,7 @@
         <v>9</v>
       </c>
       <c r="E193" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="M193" s="8"/>
       <c r="N193" s="9" t="s">
@@ -8330,7 +9195,7 @@
         <v>9</v>
       </c>
       <c r="E194" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="195" spans="1:15" ht="14">
@@ -8347,7 +9212,7 @@
         <v>9</v>
       </c>
       <c r="E195" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="196" spans="1:15" ht="14">
@@ -8364,21 +9229,21 @@
         <v>9</v>
       </c>
       <c r="E196" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="197" spans="1:15">
       <c r="A197" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B197" t="s">
+        <v>496</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D197" s="5" t="s">
         <v>506</v>
-      </c>
-      <c r="B197" t="s">
-        <v>498</v>
-      </c>
-      <c r="C197" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="D197" s="5" t="s">
-        <v>508</v>
       </c>
       <c r="E197" t="s">
         <v>246</v>
@@ -8394,16 +9259,16 @@
     </row>
     <row r="198" spans="1:15">
       <c r="A198" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B198" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C198" t="s">
         <v>214</v>
       </c>
       <c r="D198" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E198" t="s">
         <v>246</v>
@@ -8411,72 +9276,72 @@
     </row>
     <row r="199" spans="1:15" ht="14">
       <c r="A199" s="20" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B199" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C199" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D199" s="20"/>
       <c r="E199" s="19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N199">
         <v>26</v>
       </c>
       <c r="O199" s="20" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="200" spans="1:15" ht="14">
       <c r="A200" s="20" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B200" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C200" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D200" s="20"/>
       <c r="E200" s="19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O200" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="201" spans="1:15">
       <c r="A201" s="20" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B201" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D201" s="20" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E201" s="20" t="s">
         <v>128</v>
       </c>
       <c r="O201" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="202" spans="1:15">
       <c r="A202" s="20" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B202" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C202" s="20" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D202" s="20"/>
       <c r="E202" s="20" t="s">
@@ -8485,16 +9350,16 @@
     </row>
     <row r="203" spans="1:15">
       <c r="A203" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B203" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C203" s="20" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D203" s="20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E203" s="20" t="s">
         <v>246</v>
@@ -8502,13 +9367,13 @@
     </row>
     <row r="204" spans="1:15">
       <c r="A204" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B204" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C204" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E204" s="20" t="s">
         <v>246</v>
@@ -8516,12 +9381,16 @@
     </row>
     <row r="205" spans="1:15">
       <c r="A205" s="26" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="206" spans="1:15">
       <c r="A206" s="26" t="s">
-        <v>522</v>
+        <v>520</v>
+      </c>
+      <c r="E206">
+        <f>COUNTIF(E2:E196, "&lt;&gt;N/A")</f>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>